<commit_message>
Updated the backlog to reflect the product requirements
The priority has been updated to reflect what is needed
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C807D0C-E0C8-4CBA-B382-276FB3672D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76698073-90B0-4642-9E5C-649A57666C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="18576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:D15"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,6 +499,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -510,6 +513,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -521,6 +527,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
@@ -532,6 +541,9 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -543,6 +555,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -554,6 +569,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -565,6 +583,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>3</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
@@ -576,6 +597,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -587,6 +611,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>3</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
@@ -598,6 +625,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>4</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -609,6 +639,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -620,6 +653,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
@@ -631,6 +667,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>4</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>

</xml_diff>